<commit_message>
get profile of user
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
     <sheet name="Verify Email (signup)" sheetId="2" r:id="rId2"/>
     <sheet name="signin" sheetId="3" r:id="rId3"/>
     <sheet name="ResetPassword" sheetId="4" r:id="rId4"/>
+    <sheet name="Profile" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>API:</t>
   </si>
@@ -157,6 +158,24 @@
   </si>
   <si>
     <t>Lưu ý: userID lấy từ kết quả trả về ở STEP1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/users/profile</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>{
+ 'authorization': token trả ra sau khi login,
+'Content-Type': 'application/json'
+}</t>
+  </si>
+  <si>
+    <t>ressult</t>
   </si>
 </sst>
 </file>
@@ -219,6 +238,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,9 +249,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -641,6 +660,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="20227" t="32054" r="1364" b="15421"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1280160"/>
+          <a:ext cx="7886700" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -907,7 +974,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,25 +990,25 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -952,7 +1019,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -991,21 +1058,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1013,44 +1080,44 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1067,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
@@ -1078,17 +1145,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1188,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
@@ -1199,10 +1266,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1279,10 +1346,10 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -1297,10 +1364,10 @@
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
@@ -1309,12 +1376,12 @@
       <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1353,4 +1420,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
get Available money when signup
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\CNM\PROJECT\BitbucketKCoin\Documents\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\CNM\PROJECT\GitHubKcoin\Documents\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="signin" sheetId="3" r:id="rId3"/>
     <sheet name="ResetPassword" sheetId="4" r:id="rId4"/>
     <sheet name="Profile" sheetId="5" r:id="rId5"/>
+    <sheet name="Real Money" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>API:</t>
   </si>
@@ -176,6 +177,9 @@
   </si>
   <si>
     <t>ressult</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/users/realmoney</t>
   </si>
 </sst>
 </file>
@@ -708,6 +712,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="19621" t="53199" r="1894" b="39259"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="624840" y="1104900"/>
+          <a:ext cx="7894320" cy="426720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1426,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,4 +1521,62 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update API Document for verification by 2FA
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
-    <sheet name="Verify Email (signup)" sheetId="2" r:id="rId2"/>
+    <sheet name="Verify By 2FA (signup)" sheetId="2" r:id="rId2"/>
     <sheet name="signin" sheetId="3" r:id="rId3"/>
     <sheet name="ResetPassword" sheetId="4" r:id="rId4"/>
     <sheet name="Profile" sheetId="5" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>API:</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t>Vào email đã dùng để đăng ký, nhấp vào liên kết được gửi bởi email: 1412285.1412322.1412330.group@gmail.com để xác thực tài khoản</t>
-  </si>
-  <si>
-    <t>Result (nếu xác thực thành công)</t>
   </si>
   <si>
     <t>Chỉ email đã được xác thực mới có thể đăng nhập (nghĩa là thuộc tính isVerified == true)</t>
@@ -77,33 +71,6 @@
  email: req.body.email,
  password: req.body.password
 }</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/users/resetpassword/:userID</t>
-  </si>
-  <si>
-    <t>STEP1</t>
-  </si>
-  <si>
-    <t>{
- email: req.body.email
-}</t>
-  </si>
-  <si>
-    <t>STEP2</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/api/users/forgetpassword</t>
-  </si>
-  <si>
-    <t>Post</t>
-  </si>
-  <si>
-    <t>STEP3</t>
-  </si>
-  <si>
-    <t>Vào email xác thực, click vào link để vào form reset password
-(lưu ý: sửa lại link trong code back end để link tới form đăng ký trong fronend)</t>
   </si>
   <si>
     <r>
@@ -143,24 +110,6 @@
     </r>
   </si>
   <si>
-    <t>email nhận được</t>
-  </si>
-  <si>
-    <t>Kết quả trả về</t>
-  </si>
-  <si>
-    <t>{
- reset: req.body.reset (lấy từ kết quả trả về của resetToken khi gọi API ở STEP1),
- password: req.body.password (new password)
-}</t>
-  </si>
-  <si>
-    <t>Kết quả email nhận được</t>
-  </si>
-  <si>
-    <t>Lưu ý: userID lấy từ kết quả trả về ở STEP1</t>
-  </si>
-  <si>
     <t>http://localhost:8080/api/users/profile</t>
   </si>
   <si>
@@ -180,6 +129,41 @@
   </si>
   <si>
     <t>http://localhost:8080/api/users/realmoney</t>
+  </si>
+  <si>
+    <t>Result (Lưu ý kết quả của keyGoogleAuthenticator để tạo tài khoản trong Google Authenticator App)</t>
+  </si>
+  <si>
+    <t>Vào App Google Authenticator trên mobile, nhập tài khoản với tên tài khoản là email dùng để đăng ký, key là keyGoogleAuthenticator trả về sau khi đăng ký</t>
+  </si>
+  <si>
+    <t>Cứ mỗi 30 giây, App sẽ trả về một code tương ứng cho tài khoản của bạn</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/users/verify/:key</t>
+  </si>
+  <si>
+    <t>METHOD</t>
+  </si>
+  <si>
+    <t>Với key là keyGoogleAuthenticator</t>
+  </si>
+  <si>
+    <t>{
+ verifyToken: mã code nhận được từ app Google Authenticator
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/users/resetpassword</t>
+  </si>
+  <si>
+    <t>{
+ email: req.body.email,
+ password: req.body.password (new password),
+ verifyToken: mã code lấy được từ app
+                         GoogleAuthenticator tương ứng với tài khoản email 
+                         (lưu ý: mỗi 30 giây code trong App thay đổi 1 lần)
+}</t>
   </si>
 </sst>
 </file>
@@ -232,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -248,12 +232,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -305,19 +296,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -330,13 +321,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="20153" t="19529" r="1817" b="33603"/>
+        <a:srcRect l="19697" t="19798" r="1515" b="21346"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="624840" y="1112520"/>
-          <a:ext cx="7848600" cy="2651760"/>
+          <a:off x="609600" y="1104900"/>
+          <a:ext cx="7924800" cy="3329940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -353,19 +344,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>655</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -378,13 +369,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="13333" t="23031" b="54478"/>
+        <a:srcRect t="-1" b="44016"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1920240" y="358140"/>
-          <a:ext cx="8717280" cy="1272540"/>
+          <a:off x="2004061" y="0"/>
+          <a:ext cx="3093719" cy="3079135"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -396,19 +387,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>488738</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -421,13 +412,56 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="4040" b="83165"/>
+        <a:srcRect b="34470"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2019300" y="1836420"/>
-          <a:ext cx="10058400" cy="723900"/>
+          <a:off x="2019301" y="3299460"/>
+          <a:ext cx="2995717" cy="3489960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1996440</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="19849" t="19529" r="1743" b="39125"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1996440" y="8046720"/>
+          <a:ext cx="7886700" cy="2339340"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,18 +570,18 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1348740</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -560,99 +594,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="13182" t="23300" r="682" b="52996"/>
+        <a:srcRect l="19621" t="19394" r="1515" b="41279"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1554480" y="4945380"/>
-          <a:ext cx="8663940" cy="1341120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="20152" t="19124" r="985" b="35623"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1554480" y="1112520"/>
-          <a:ext cx="7932420" cy="2560320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="20151" t="19798" r="1516" b="34141"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1546860" y="7795260"/>
-          <a:ext cx="7879080" cy="2606040"/>
+          <a:off x="1554480" y="1844040"/>
+          <a:ext cx="7932420" cy="2225040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1023,15 +971,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:S1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="24.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1043,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -1072,20 +1020,75 @@
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:S1"/>
+    <mergeCell ref="A4:A22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
@@ -1098,87 +1101,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:1" ht="242.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:M1"/>
+  <mergeCells count="2">
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="C23:F23"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1198,7 +1228,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1211,7 +1241,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1219,7 +1249,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1227,15 +1257,15 @@
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1291,7 +1321,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1305,52 +1335,49 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -1385,89 +1412,9 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C25:F25"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1489,31 +1436,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1527,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1538,26 +1485,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
admin: get list transaction
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ResetPassword" sheetId="4" r:id="rId4"/>
     <sheet name="Profile" sheetId="5" r:id="rId5"/>
     <sheet name="Real Money" sheetId="6" r:id="rId6"/>
+    <sheet name="Mục 4.4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>API:</t>
   </si>
@@ -171,6 +172,50 @@
  password: req.body.password,
  verifyToken: lấy từ App
 }</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/admin/transactionInfo</t>
+  </si>
+  <si>
+    <t>Table theo như sau</t>
+  </si>
+  <si>
+    <t>Hash Transaction</t>
+  </si>
+  <si>
+    <t>data.listResult[i].hash</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>data.listResult[i].time</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>data.listResult[i].state</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>data.listResult[i].inputs
+(lưu ý: đây là 1 list, phải hiện tất cả những thông tin trong list đó(hình bên), hiện sao cho đẹp nhé :)</t>
+  </si>
+  <si>
+    <t>data.listResult[i].outputs
+(lưu ý: đây là 1 list, phải hiện tất cả những thông tin trong list đó(hình bên), hiện sao cho đẹp nhé :)</t>
+  </si>
+  <si>
+    <t>Link tham khảo giao diện tương tự như thầy:</t>
+  </si>
+  <si>
+    <t>https://kcoin.club/#/blocks/000194f14791840ea92b18b543c590f2833d3f69d6eb1c3c67b99214bc375343</t>
   </si>
 </sst>
 </file>
@@ -210,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -218,12 +263,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -251,6 +311,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -715,6 +782,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>716280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>263726</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24470" t="34613" r="3030" b="4647"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="1082040"/>
+          <a:ext cx="7373186" cy="3474720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -980,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,4 +1648,106 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="216" x14ac:dyDescent="0.3">
+      <c r="K6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update 4.4: chỉ hiện thông tin của hệ thống chứ ko hiển thị toàn bộ
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>API:</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>https://kcoin.club/#/blocks/000194f14791840ea92b18b543c590f2833d3f69d6eb1c3c67b99214bc375343</t>
+  </si>
+  <si>
+    <t>Hiện thêm Email của User đi kèm với output nữa</t>
   </si>
 </sst>
 </file>
@@ -303,6 +306,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,13 +321,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -788,18 +791,18 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>716280</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>263726</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -812,13 +815,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="24470" t="34613" r="3030" b="4647"/>
+        <a:srcRect l="23334" t="32189" r="2273" b="5993"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="617220" y="1082040"/>
-          <a:ext cx="7373186" cy="3474720"/>
+          <a:off x="617220" y="1112520"/>
+          <a:ext cx="7482840" cy="3497580"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1112,25 +1115,25 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1149,63 +1152,63 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="13"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="13"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="13"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
+      <c r="A20" s="13"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+      <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
+      <c r="A22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1245,30 +1248,30 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11"/>
@@ -1289,12 +1292,12 @@
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1349,17 +1352,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1652,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,36 +1704,36 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="216" x14ac:dyDescent="0.3">
-      <c r="K6" s="13" t="s">
+    <row r="6" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="K6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1745,7 +1748,17 @@
         <v>43</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K11:M11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
statistic: 4.5 - get total by Address in System
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Profile" sheetId="5" r:id="rId5"/>
     <sheet name="Real Money" sheetId="6" r:id="rId6"/>
     <sheet name="Mục 4.4" sheetId="7" r:id="rId7"/>
+    <sheet name="Mục 4.5" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>API:</t>
   </si>
@@ -219,6 +220,33 @@
   </si>
   <si>
     <t>Hiện thêm Email của User đi kèm với output nữa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/admin/totalByAddress</t>
+  </si>
+  <si>
+    <t>Header &amp; Body</t>
+  </si>
+  <si>
+    <t>Truyền như thống kê total, headers có token, contentType, Body có limit và offset</t>
+  </si>
+  <si>
+    <t>Các cột trong table hiển thị theo thứ tự sau</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Actual Balance</t>
+  </si>
+  <si>
+    <t>Available Balance</t>
+  </si>
+  <si>
+    <t>Reference User</t>
   </si>
 </sst>
 </file>
@@ -833,6 +861,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24015" t="31784" r="17424" b="8687"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="548640"/>
+          <a:ext cx="5890260" cy="3368040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1657,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1763,4 +1839,79 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pagination for transaction list
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -817,20 +817,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -843,13 +843,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="23334" t="32189" r="2273" b="5993"/>
+        <a:srcRect l="23409" t="32054" r="13333" b="5993"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="617220" y="1112520"/>
-          <a:ext cx="7482840" cy="3497580"/>
+          <a:off x="586740" y="563880"/>
+          <a:ext cx="6362700" cy="3505200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1731,23 +1731,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1755,85 +1755,85 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="K5" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="I6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="K6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K8" s="3" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K9" t="s">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K11" s="14" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1858,7 +1858,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B1" t="s">
@@ -1866,7 +1866,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
@@ -1882,7 +1882,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="N4" t="s">

</xml_diff>

<commit_message>
Get transaction history for user, delete initialized transaction
</commit_message>
<xml_diff>
--- a/Documents/API/UserAPI.xlsx
+++ b/Documents/API/UserAPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Mục 4.5" sheetId="8" r:id="rId9"/>
     <sheet name="SendMoney" sheetId="9" r:id="rId10"/>
     <sheet name="VerifyTransaction" sheetId="11" r:id="rId11"/>
+    <sheet name="TransactionHistoryOfUser" sheetId="12" r:id="rId12"/>
+    <sheet name="DeleteInitializedTransaction" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
   <si>
     <t>API:</t>
   </si>
@@ -292,6 +294,51 @@
  verifyToken: req.body.verifyToken(lấy từ app),
 verifyValue: req.body.verifyValue(true: nếu người dùng click button đồng ý, false: nếu người dùng click button từ chối )
 }</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/transactions/history</t>
+  </si>
+  <si>
+    <t>Bao gồm 2 bảng</t>
+  </si>
+  <si>
+    <t>listTranSend  : Bảng chứa thông tin rút tiền</t>
+  </si>
+  <si>
+    <t>Hash transaction</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Trong bảng này transaction nào có trạng thái là "initialized" (trạng thái khởi tạo của transaction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nếu người dùng nhấp chọn "Delete" thì sẽ gọi đến phương thức GET của API (http://localhost:8080/api/transactions/delete/:key)</t>
+  </si>
+  <si>
+    <t>listTranReceive : Bảng chứa thông tin nạp tiền</t>
+  </si>
+  <si>
+    <t>Sender address</t>
+  </si>
+  <si>
+    <t>Output index</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/api/transactions/delete/:key</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thì sẽ có thêm nút "Delete" trên dòng chứa thông tin transaction này để người dùng có thể xóa nếu muốn và trong danh sách giá trị của transaction này sẽ có thêm thuộc tính </t>
+  </si>
+  <si>
+    <t>auth: keyGoogleAuthenticator để truyền cho key trong API (http://localhost:8080/api/transactions/delete/:key)</t>
+  </si>
+  <si>
+    <t>Result (success)</t>
   </si>
 </sst>
 </file>
@@ -331,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -354,12 +401,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -387,6 +460,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -395,14 +477,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -598,6 +686,166 @@
         <a:xfrm>
           <a:off x="1228725" y="7515225"/>
           <a:ext cx="4429743" cy="1390844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>277399</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>181612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06DBA01-C4C4-4BE9-86C7-7B19125AFE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2095500"/>
+          <a:ext cx="8411749" cy="4563112"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>220326</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9872</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B444DC10-D2E2-4342-9EB5-72C2847B6904}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6667500"/>
+          <a:ext cx="8964276" cy="2486372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>410221</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19159</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D940032-E00B-41C9-B0A2-725865EC481B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="981075" y="2286000"/>
+          <a:ext cx="4629796" cy="781159"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1521,25 +1769,25 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1558,63 +1806,63 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="16"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="16"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="16"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1700,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1959,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1729,7 +1977,7 @@
       <c r="A5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1756,7 +2004,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1764,7 +2012,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1784,6 +2032,222 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12" s="13"/>
+      <c r="N12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N13" s="19"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="21" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="O21" s="18"/>
+      <c r="P21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q21" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="T21" s="18"/>
+      <c r="U21" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N22" s="21"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1826,30 +2290,30 @@
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11"/>
@@ -1870,12 +2334,12 @@
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1930,17 +2394,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2327,11 +2791,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2347,7 +2811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>